<commit_message>
Updated Excel report : 29.06 && Added python input/output tasks
</commit_message>
<xml_diff>
--- a/2024-УП-task_time_manager_2гр_Большаков.xlsx
+++ b/2024-УП-task_time_manager_2гр_Большаков.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\UP\AB_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45A9E1C-D254-4C2E-9906-FC598DB4560B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DB1AC7-9504-4287-A601-FA4D29B99712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManager" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>№ за день</t>
   </si>
@@ -148,9 +148,6 @@
     <t xml:space="preserve">Установил питон и настроил окружение </t>
   </si>
   <si>
-    <t>Изучение введения</t>
-  </si>
-  <si>
     <t xml:space="preserve">Понял как устрое курс и хендбук </t>
   </si>
   <si>
@@ -166,16 +163,49 @@
     <t>Научился пользоваться циклами for и while, а также разобрался с range()</t>
   </si>
   <si>
-    <t>Изучение Условный оператор</t>
-  </si>
-  <si>
-    <t>Изучение Циклы</t>
-  </si>
-  <si>
-    <t>Изучение Вложенные циклы</t>
-  </si>
-  <si>
     <t>Научился использовать вложенные циклы</t>
+  </si>
+  <si>
+    <t>Python Изучение Условный оператор</t>
+  </si>
+  <si>
+    <t>куср Python Изучение введения</t>
+  </si>
+  <si>
+    <t>куср Python Изучение Циклы</t>
+  </si>
+  <si>
+    <t>куср Python Изучение Вложенные циклы</t>
+  </si>
+  <si>
+    <t>курс Python Изучение Множества, словари</t>
+  </si>
+  <si>
+    <t>курс Python Изучение Строки, кортежи, списки</t>
+  </si>
+  <si>
+    <t>курс Python Изучение Списочные выражения. Модель памяти для типов языка Python</t>
+  </si>
+  <si>
+    <t>курс Python Изучение Встроенные возможности по работе с коллекциями</t>
+  </si>
+  <si>
+    <t>курс Python Изучение Потоковый ввод/вывод. Работа с текстовыми файлами. JSON</t>
+  </si>
+  <si>
+    <t>Разобрался с данной темой</t>
+  </si>
+  <si>
+    <t>Разобрался со словарами и множетсвами</t>
+  </si>
+  <si>
+    <t>Изучил данную тему</t>
+  </si>
+  <si>
+    <t>Изучил встроенные вохможности по работе с коллекциями в Python</t>
+  </si>
+  <si>
+    <t>Разобрался с потоковым вводом выводом. И разобрадся как работать с Json файлами</t>
   </si>
 </sst>
 </file>
@@ -604,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -790,7 +820,7 @@
         <v>45468.840277777781</v>
       </c>
       <c r="E8" s="11">
-        <f t="shared" ref="E8:E23" si="1">D8-C8</f>
+        <f t="shared" ref="E8:E21" si="1">D8-C8</f>
         <v>7.6388888890505768E-2</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -1054,7 +1084,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C20" s="16">
         <v>45471.402777777781</v>
@@ -1067,7 +1097,7 @@
         <v>2.7777777773735579E-2</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="10"/>
     </row>
@@ -1076,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="16">
         <v>45471.430555555555</v>
@@ -1089,7 +1119,7 @@
         <v>4.8611111109494232E-2</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="10"/>
     </row>
@@ -1111,7 +1141,7 @@
         <v>8.3333333335758653E-2</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="10"/>
     </row>
@@ -1120,7 +1150,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="16">
         <v>45471.645833333336</v>
@@ -1133,16 +1163,16 @@
         <v>4.8611111109494232E-2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>5</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24" s="16">
         <v>45471.694444444445</v>
@@ -1155,32 +1185,125 @@
         <v>4.8611111109494232E-2</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G24" s="21">
         <f>SUM(E19:E24)</f>
         <v>0.28472222221898846</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="13"/>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="13"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="13"/>
-      <c r="F29" s="13"/>
+    <row r="25" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>6</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="16">
+        <v>45472.375</v>
+      </c>
+      <c r="D25" s="16">
+        <v>45472.416666666664</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" ref="E25:E29" si="2">D25-C25</f>
+        <v>4.1666666664241347E-2</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>6</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="16">
+        <v>45472.416666666664</v>
+      </c>
+      <c r="D26" s="16">
+        <v>45472.465277777781</v>
+      </c>
+      <c r="E26" s="11">
+        <f t="shared" si="2"/>
+        <v>4.8611111116770189E-2</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>6</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="16">
+        <v>45472.465277777781</v>
+      </c>
+      <c r="D27" s="16">
+        <v>45472.527777777781</v>
+      </c>
+      <c r="E27" s="11">
+        <f t="shared" si="2"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>6</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="16">
+        <v>45472.527777777781</v>
+      </c>
+      <c r="D28" s="16">
+        <v>45472.590277777781</v>
+      </c>
+      <c r="E28" s="11">
+        <f t="shared" si="2"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>6</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="16">
+        <v>45472.590277777781</v>
+      </c>
+      <c r="D29" s="16">
+        <v>45472.631944444445</v>
+      </c>
+      <c r="E29" s="11">
+        <f t="shared" si="2"/>
+        <v>4.1666666664241347E-2</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="21">
+        <f>SUM(E25:E29)</f>
+        <v>0.25694444444525288</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="13"/>

</xml_diff>

<commit_message>
Added python def tasks (4.1) & small changes in excel report
</commit_message>
<xml_diff>
--- a/2024-УП-task_time_manager_2гр_Большаков.xlsx
+++ b/2024-УП-task_time_manager_2гр_Большаков.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\UP\AB_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DB1AC7-9504-4287-A601-FA4D29B99712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C429C48-274A-4E06-A8E2-40CDB250D7DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManager" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>№ за день</t>
   </si>
@@ -154,18 +154,6 @@
     <t>Изучение Ввод и вывод данных. Операции с числами, строками. Форматирование</t>
   </si>
   <si>
-    <t>Научился вводить и выводить информацию, разобрался в базовых арифметических операторах, а также научился форматировать вывод информации</t>
-  </si>
-  <si>
-    <t>Научился использовать операторы ветвления</t>
-  </si>
-  <si>
-    <t>Научился пользоваться циклами for и while, а также разобрался с range()</t>
-  </si>
-  <si>
-    <t>Научился использовать вложенные циклы</t>
-  </si>
-  <si>
     <t>Python Изучение Условный оператор</t>
   </si>
   <si>
@@ -193,19 +181,37 @@
     <t>курс Python Изучение Потоковый ввод/вывод. Работа с текстовыми файлами. JSON</t>
   </si>
   <si>
-    <t>Разобрался с данной темой</t>
-  </si>
-  <si>
-    <t>Разобрался со словарами и множетсвами</t>
-  </si>
-  <si>
-    <t>Изучил данную тему</t>
-  </si>
-  <si>
-    <t>Изучил встроенные вохможности по работе с коллекциями в Python</t>
-  </si>
-  <si>
-    <t>Разобрался с потоковым вводом выводом. И разобрадся как работать с Json файлами</t>
+    <t>Научился вводить и выводить информацию, разобрался в базовых арифметических операторах, а также научился форматировать вывод информации, решил 20 задач после темы</t>
+  </si>
+  <si>
+    <t>Научился использовать операторы ветвления, решил 20 задач после темы</t>
+  </si>
+  <si>
+    <t>Научился пользоваться циклами for и while, а также разобрался с range(), решил 17 задач после темы</t>
+  </si>
+  <si>
+    <t>Научился использовать вложенные циклы, решил 14 задач после темы</t>
+  </si>
+  <si>
+    <t>Разобрался с данной темой, решил 15 задач после темы</t>
+  </si>
+  <si>
+    <t>Разобрался со словарами и множетсвами, решил 16 задач после темы</t>
+  </si>
+  <si>
+    <t>Изучил данную тему, решил 10 задач после темы</t>
+  </si>
+  <si>
+    <t>Изучил встроенные вохможности по работе с коллекциями в Python, решил 14 задач после темы</t>
+  </si>
+  <si>
+    <t>Разобрался с потоковым вводом выводом. И разобрадся как работать с Json файлами, решил 11 задач после темы</t>
+  </si>
+  <si>
+    <t>Заполнение отчета</t>
+  </si>
+  <si>
+    <t>Заполнил в отчете требуемые пункты</t>
   </si>
 </sst>
 </file>
@@ -634,8 +640,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="102" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1084,7 +1090,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" s="16">
         <v>45471.402777777781</v>
@@ -1119,7 +1125,7 @@
         <v>4.8611111109494232E-2</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G21" s="10"/>
     </row>
@@ -1128,7 +1134,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C22" s="16">
         <v>45471.479166666664</v>
@@ -1141,7 +1147,7 @@
         <v>8.3333333335758653E-2</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G22" s="10"/>
     </row>
@@ -1150,7 +1156,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C23" s="16">
         <v>45471.645833333336</v>
@@ -1163,7 +1169,7 @@
         <v>4.8611111109494232E-2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -1172,7 +1178,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C24" s="16">
         <v>45471.694444444445</v>
@@ -1185,7 +1191,7 @@
         <v>4.8611111109494232E-2</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G24" s="21">
         <f>SUM(E19:E24)</f>
@@ -1197,7 +1203,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C25" s="16">
         <v>45472.375</v>
@@ -1206,7 +1212,7 @@
         <v>45472.416666666664</v>
       </c>
       <c r="E25" s="11">
-        <f t="shared" ref="E25:E29" si="2">D25-C25</f>
+        <f t="shared" ref="E25:E30" si="2">D25-C25</f>
         <v>4.1666666664241347E-2</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -1219,7 +1225,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C26" s="16">
         <v>45472.416666666664</v>
@@ -1236,12 +1242,12 @@
       </c>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>6</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C27" s="16">
         <v>45472.465277777781</v>
@@ -1263,7 +1269,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C28" s="16">
         <v>45472.527777777781</v>
@@ -1285,7 +1291,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" s="16">
         <v>45472.590277777781</v>
@@ -1300,14 +1306,32 @@
       <c r="F29" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="21">
-        <f>SUM(E25:E29)</f>
-        <v>0.25694444444525288</v>
-      </c>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="A30" s="9">
+        <v>6</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="16">
+        <v>45472.666666666664</v>
+      </c>
+      <c r="D30" s="16">
+        <v>45472.777777777781</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" si="2"/>
+        <v>0.11111111111677019</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="21">
+        <f>SUM(E25:E30)</f>
+        <v>0.36805555556202307</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="13"/>

</xml_diff>

<commit_message>
Added python lambda tasks (4.2) & edited excel report
</commit_message>
<xml_diff>
--- a/2024-УП-task_time_manager_2гр_Большаков.xlsx
+++ b/2024-УП-task_time_manager_2гр_Большаков.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\UP\AB_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C429C48-274A-4E06-A8E2-40CDB250D7DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FC7BD1-0B7F-488C-B112-1DFC10C3458D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManager" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>№ за день</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>Заполнил в отчете требуемые пункты</t>
+  </si>
+  <si>
+    <t>Разобрался с использованием функция в Python, решил 10 задач</t>
+  </si>
+  <si>
+    <t>курc Python изучение Функции. Области видимости. Передача параметров в функции</t>
+  </si>
+  <si>
+    <t>Курc Python Позиционные и именованные аргументы. Функции высших порядков. Лямбда-функции</t>
+  </si>
+  <si>
+    <t>Разобрался как устроены лямбда функции и как работаь с позиционными и именованными аргументами, решил 8 задач</t>
   </si>
 </sst>
 </file>
@@ -294,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -358,11 +370,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,6 +443,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,8 +669,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="102" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="102" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1212,7 +1241,7 @@
         <v>45472.416666666664</v>
       </c>
       <c r="E25" s="11">
-        <f t="shared" ref="E25:E30" si="2">D25-C25</f>
+        <f t="shared" ref="E25:E32" si="2">D25-C25</f>
         <v>4.1666666664241347E-2</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -1333,13 +1362,47 @@
         <v>0.36805555556202307</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="13"/>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="13"/>
-      <c r="F32" s="13"/>
+    <row r="31" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="25">
+        <v>7</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="16">
+        <v>45474.375</v>
+      </c>
+      <c r="D31" s="16">
+        <v>45474.423611111109</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="2"/>
+        <v>4.8611111109494232E-2</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="25">
+        <v>7</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="16">
+        <v>45474.423611111109</v>
+      </c>
+      <c r="D32" s="16">
+        <v>45474.5</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="2"/>
+        <v>7.6388888890505768E-2</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="13"/>

</xml_diff>

<commit_message>
Added python tasks (5.1, 5.2, 5.3) & edited Excel report
</commit_message>
<xml_diff>
--- a/2024-УП-task_time_manager_2гр_Большаков.xlsx
+++ b/2024-УП-task_time_manager_2гр_Большаков.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\UP\AB_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FC7BD1-0B7F-488C-B112-1DFC10C3458D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB9649D-DD7A-4574-861F-19A33CB82326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3150" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManager" sheetId="2" r:id="rId1"/>
+    <sheet name="Курс Python" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>№ за день</t>
   </si>
@@ -224,6 +225,54 @@
   </si>
   <si>
     <t>Разобрался как устроены лямбда функции и как работаь с позиционными и именованными аргументами, решил 8 задач</t>
+  </si>
+  <si>
+    <t>курс Python изучение Рекурсия. Декораторы. Генераторы</t>
+  </si>
+  <si>
+    <t>Работа над отчетом</t>
+  </si>
+  <si>
+    <t>Разобрался и научился пользоваться декораторами и генераторами,решил 9 задач</t>
+  </si>
+  <si>
+    <t>Исправил некоторые недочеты</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.1</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.2</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.3</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.4</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.1</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.2</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.3</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.4</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.5</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/4.1</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/4.2</t>
+  </si>
+  <si>
+    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/4.3</t>
   </si>
 </sst>
 </file>
@@ -306,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -370,22 +419,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -443,12 +481,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,6 +497,545 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA9EEA0-19FB-4DE6-A5EB-022D711889A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95250" y="28575"/>
+          <a:ext cx="8658225" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>360838</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5392206-B91A-4E7B-B578-7332F1DDB8FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1133475"/>
+          <a:ext cx="8895238" cy="561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>65524</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5CD9C54-ECFC-4375-BBB5-9DC08E76097F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2105025"/>
+          <a:ext cx="9209524" cy="552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>322743</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{921D5193-C31F-4755-8178-6F3CFEE66517}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3076575"/>
+          <a:ext cx="8857143" cy="542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>36952</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF7E40B9-DED4-4BA7-BF0E-D2858484B31B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4048125"/>
+          <a:ext cx="9180952" cy="561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>208457</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123749</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFBC3E0A-8A08-4539-989D-332A405ADCBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5181600"/>
+          <a:ext cx="8742857" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>313219</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>9443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8ABFD41-3C7B-4549-8260-5FCBEFAA6DB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6153150"/>
+          <a:ext cx="8847619" cy="657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>341790</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>104701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F8C345A-20B6-45B4-9E86-BDA472B9169E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7286625"/>
+          <a:ext cx="8876190" cy="590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>379886</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>28490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD93AB14-DD8B-4524-9D11-A6F5CAD3F311}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8420100"/>
+          <a:ext cx="8914286" cy="676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>65600</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>142796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C6DC97-E2FD-41AC-B98D-BEBB9EAD5DC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9553575"/>
+          <a:ext cx="8600000" cy="628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>141790</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>152300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2771116-C296-4F09-B3E3-3F9D6909EE3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10525125"/>
+          <a:ext cx="8676190" cy="800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>341790</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>57062</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7D044B5-6A2D-42BB-966F-A93702F8EBE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="11658600"/>
+          <a:ext cx="8876190" cy="704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -669,8 +1241,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="102" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="102" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1241,7 +1813,7 @@
         <v>45472.416666666664</v>
       </c>
       <c r="E25" s="11">
-        <f t="shared" ref="E25:E32" si="2">D25-C25</f>
+        <f t="shared" ref="E25:E34" si="2">D25-C25</f>
         <v>4.1666666664241347E-2</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -1363,105 +1935,146 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="25">
+      <c r="A31" s="9">
         <v>7</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="16">
         <v>45474.375</v>
       </c>
       <c r="D31" s="16">
-        <v>45474.423611111109</v>
+        <v>45474.444444444445</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="2"/>
-        <v>4.8611111109494232E-2</v>
-      </c>
-      <c r="F31" s="26" t="s">
+        <v>6.9444444445252884E-2</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>64</v>
       </c>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="25">
+      <c r="A32" s="9">
         <v>7</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C32" s="16">
-        <v>45474.423611111109</v>
+        <v>45474.444444444445</v>
       </c>
       <c r="D32" s="16">
-        <v>45474.5</v>
+        <v>45474.520833333336</v>
       </c>
       <c r="E32" s="11">
         <f t="shared" si="2"/>
         <v>7.6388888890505768E-2</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="13"/>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="13"/>
-      <c r="F34" s="13"/>
-    </row>
-    <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>7</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="16">
+        <v>45474.520833333336</v>
+      </c>
+      <c r="D33" s="16">
+        <v>45474.548611111109</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="2"/>
+        <v>2.7777777773735579E-2</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>7</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="16">
+        <v>45474.625</v>
+      </c>
+      <c r="D34" s="16">
+        <v>45474.722222222219</v>
+      </c>
+      <c r="E34" s="11">
+        <f t="shared" si="2"/>
+        <v>9.7222222218988463E-2</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" s="21">
+        <f>SUM(E31:E34)</f>
+        <v>0.27083333332848269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="13"/>
       <c r="F35" s="13"/>
     </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="13"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="13"/>
       <c r="F37" s="13"/>
     </row>
-    <row r="38" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="13"/>
       <c r="F38" s="13"/>
     </row>
-    <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="13"/>
       <c r="F39" s="13"/>
     </row>
-    <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="13"/>
       <c r="F40" s="13"/>
     </row>
-    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="13"/>
       <c r="F41" s="13"/>
     </row>
-    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13"/>
       <c r="F42" s="13"/>
     </row>
-    <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="24"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="24"/>
       <c r="F44" s="13"/>
     </row>
-    <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F45" s="13"/>
     </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F46" s="13"/>
     </row>
-    <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F47" s="13"/>
     </row>
-    <row r="48" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F48" s="13"/>
     </row>
     <row r="49" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1473,4 +2086,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F2CB36-37D6-4F5C-A5E8-8F0B95A87B2D}">
+  <dimension ref="A6:A78"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added c++ Json console task & edited Excel report
</commit_message>
<xml_diff>
--- a/2024-УП-task_time_manager_2гр_Большаков.xlsx
+++ b/2024-УП-task_time_manager_2гр_Большаков.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\UP\AB_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB9649D-DD7A-4574-861F-19A33CB82326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CE301E-48E2-42CC-84A5-AC58E3E3A78D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManager" sheetId="2" r:id="rId1"/>
-    <sheet name="Курс Python" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>№ за день</t>
   </si>
@@ -239,40 +238,22 @@
     <t>Исправил некоторые недочеты</t>
   </si>
   <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.1</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.2</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.3</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/2.4</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.1</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.2</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.3</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.4</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/3.5</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/4.1</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/4.2</t>
-  </si>
-  <si>
-    <t>Ссылка на Git : https://github.com/ArpiJokle/AB_Practice/tree/master/Python/4.3</t>
+    <t>курс Python изучение Объектная модель Python. Классы, поля и методы</t>
+  </si>
+  <si>
+    <t>курс Python изучение Волшебные методы, переопределение методов. Наследование</t>
+  </si>
+  <si>
+    <t>курс Python изучение Модель исключений Python. Try, except, else, finally. Модули</t>
+  </si>
+  <si>
+    <t>курс Python изучение Модули math и numpy</t>
+  </si>
+  <si>
+    <t>Выполнение практического задания по работе с Json форматами в c++</t>
+  </si>
+  <si>
+    <t>Освоил на практике устройство Json файлов, а также закрепил знания по использованию библиотеки для работы в с++ с Json файлами</t>
   </si>
 </sst>
 </file>
@@ -355,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -419,11 +400,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -437,16 +472,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -462,7 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -476,12 +501,69 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,23 +585,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>37354</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>653677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4248898</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1019697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA9EEA0-19FB-4DE6-A5EB-022D711889A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33690CC0-33EB-404B-8C1F-08B10EC8E095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -541,8 +623,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="95250" y="28575"/>
-          <a:ext cx="8658225" cy="752475"/>
+          <a:off x="5266766" y="11570074"/>
+          <a:ext cx="4211544" cy="366020"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -553,23 +635,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28015</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>373530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>360838</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76130</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4388970</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>649008</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5392206-B91A-4E7B-B578-7332F1DDB8FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C345284E-A333-4130-9BEB-D22FF96BFA05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -585,8 +667,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1133475"/>
-          <a:ext cx="8895238" cy="561905"/>
+          <a:off x="5257427" y="12466545"/>
+          <a:ext cx="4360955" cy="275478"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -597,23 +679,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>37353</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>420220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>65524</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>66606</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4426323</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>700367</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5CD9C54-ECFC-4375-BBB5-9DC08E76097F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63B010FD-56C4-484C-97B1-FEDC36E8576A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -629,8 +711,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2105025"/>
-          <a:ext cx="9209524" cy="552381"/>
+          <a:off x="5266765" y="13334999"/>
+          <a:ext cx="4388970" cy="280147"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -641,23 +723,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28015</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>364191</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>322743</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57082</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4473015</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>636626</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{921D5193-C31F-4755-8178-6F3CFEE66517}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDBCC059-8764-4027-B99D-DE4F2DC6B3B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -673,8 +755,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3076575"/>
-          <a:ext cx="8857143" cy="542857"/>
+          <a:off x="5257427" y="14231470"/>
+          <a:ext cx="4445000" cy="272435"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -685,23 +767,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9338</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>270810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>36952</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76130</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4398308</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>539430</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF7E40B9-DED4-4BA7-BF0E-D2858484B31B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63663880-7CD3-4951-9F12-94198140C263}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -717,8 +799,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4048125"/>
-          <a:ext cx="9180952" cy="561905"/>
+          <a:off x="5238750" y="15137281"/>
+          <a:ext cx="4388970" cy="268620"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -729,23 +811,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>242794</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>208457</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>123749</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4342284</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>541618</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFBC3E0A-8A08-4539-989D-332A405ADCBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27D1B866-CE26-4AFF-A294-FEBC2BE869F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -761,8 +843,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="5181600"/>
-          <a:ext cx="8742857" cy="609524"/>
+          <a:off x="5285441" y="15538823"/>
+          <a:ext cx="4286255" cy="298824"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -773,23 +855,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>65368</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>280146</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>313219</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>9443</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4435662</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>604743</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8ABFD41-3C7B-4549-8260-5FCBEFAA6DB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BBE9EEA-DA02-436B-9817-F56B8CC30BB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,8 +887,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6153150"/>
-          <a:ext cx="8847619" cy="657143"/>
+          <a:off x="5294780" y="16304558"/>
+          <a:ext cx="4370294" cy="324597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -817,23 +899,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>382868</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>341790</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>104701</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4407647</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>672353</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F8C345A-20B6-45B4-9E86-BDA472B9169E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{678D2285-C7EF-4938-9D25-0419745CD87B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -849,8 +931,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="7286625"/>
-          <a:ext cx="8876190" cy="590476"/>
+          <a:off x="5285441" y="17145000"/>
+          <a:ext cx="4351618" cy="289485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -861,23 +943,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9338</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>382867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>379886</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>28490</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4441196</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>719044</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD93AB14-DD8B-4524-9D11-A6F5CAD3F311}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B6363C-1553-45F2-88C2-ADA5E71B81C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -893,8 +975,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="8420100"/>
-          <a:ext cx="8914286" cy="676190"/>
+          <a:off x="5238750" y="17938749"/>
+          <a:ext cx="4431858" cy="336177"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -905,23 +987,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>295932</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>65600</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>142796</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4407647</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>609895</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C6DC97-E2FD-41AC-B98D-BEBB9EAD5DC0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD017ABD-DB45-4C27-ACE5-A6D74944D731}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -937,8 +1019,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="9553575"/>
-          <a:ext cx="8600000" cy="628571"/>
+          <a:off x="5341471" y="18879020"/>
+          <a:ext cx="4295588" cy="313963"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -949,23 +1031,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>93380</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>372460</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>141790</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>152300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4426321</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>771985</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2771116-C296-4F09-B3E3-3F9D6909EE3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{530AF9E0-0069-4313-8DA6-AB08F1C3C870}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -981,8 +1063,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="10525125"/>
-          <a:ext cx="8676190" cy="800000"/>
+          <a:off x="5322792" y="19711945"/>
+          <a:ext cx="4332941" cy="399525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,23 +1075,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>93383</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>444032</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>341790</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>57062</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4435662</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>788805</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7D044B5-6A2D-42BB-966F-A93702F8EBE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{696507FF-D553-4075-9486-E87CFA8B7A68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1025,8 +1107,184 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="11658600"/>
-          <a:ext cx="8876190" cy="704762"/>
+          <a:off x="5322795" y="21314988"/>
+          <a:ext cx="4342279" cy="344773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>196104</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>326839</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4191542</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>646242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51634626-B302-4913-9CFE-A5A4E6B7644D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5425516" y="22038236"/>
+          <a:ext cx="3995438" cy="319403"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>46691</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>270808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4207207</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>753725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B5304C-6B1F-4191-BA27-7605CEBD252A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5276103" y="22916029"/>
+          <a:ext cx="4160516" cy="482917"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177426</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>233457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4283418</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>722553</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480B67E4-AD63-459D-B6CD-2C5BA6E63714}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5406838" y="24017942"/>
+          <a:ext cx="4105992" cy="489096"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>280146</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>121398</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4114013</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>389142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98EBE9C3-BD98-49DE-90A3-A1C653F0C40A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5509558" y="24793016"/>
+          <a:ext cx="3833867" cy="267744"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1241,8 +1499,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="102" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="102" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1509,7 @@
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="67.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1322,844 +1580,851 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="25">
         <v>45467.694444444445</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="25">
         <v>45467.798611111109</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="26">
         <f t="shared" si="0"/>
         <v>0.10416666666424135</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="27">
         <f>SUM(E2:E4)</f>
         <v>0.25694444443797693</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="21">
         <v>45468.541666666664</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="21">
         <v>45468.569444444445</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="22">
         <f t="shared" si="0"/>
         <v>2.7777777781011537E-2</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>2</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>45468.569444444445</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>45468.680555555555</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="11">
         <f t="shared" si="0"/>
         <v>0.11111111110949423</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>45468.680555555555</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="12">
         <v>45468.722222222219</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
         <v>2</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="31">
         <v>45468.763888888891</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="31">
         <v>45468.840277777781</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="32">
         <f t="shared" ref="E8:E21" si="1">D8-C8</f>
         <v>7.6388888890505768E-2</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="33">
         <f>SUM(E5:E8)</f>
         <v>0.25694444444525288</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="A9" s="19">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="28">
         <v>45469.375</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="28">
         <v>45469.416666666664</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="22">
         <f t="shared" si="1"/>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="12">
         <v>45469.416666666664</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="12">
         <v>45469.5</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="8">
         <f t="shared" si="1"/>
         <v>8.3333333335758653E-2</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="6">
         <v>3</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="12">
         <v>45469.5</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="12">
         <v>45469.541666666664</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <f t="shared" si="1"/>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="12">
         <v>45469.625</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="12">
         <v>45469.666666666664</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="8">
         <f t="shared" si="1"/>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="31">
         <v>45469.666666666664</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="31">
         <v>45469.708333333336</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="32">
         <f t="shared" si="1"/>
         <v>4.1666666671517305E-2</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="34">
         <f>SUM(E9:E13)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+      <c r="A14" s="19">
         <v>4</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="28">
         <v>45470.375</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="28">
         <v>45470.4375</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="22">
         <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>4</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="12">
         <v>45470.4375</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="12">
         <v>45470.493055555555</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="8">
         <f t="shared" si="1"/>
         <v>5.5555555554747116E-2</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
+      <c r="A16" s="6">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="12">
         <v>45470.493055555555</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="12">
         <v>45470.541666666664</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="8">
         <f t="shared" si="1"/>
         <v>4.8611111109494232E-2</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>4</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="12">
         <v>45470.625</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="12">
         <v>45470.673611111109</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="8">
         <f t="shared" si="1"/>
         <v>4.8611111109494232E-2</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
         <v>4</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="31">
         <v>45470.673611111109</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="31">
         <v>45470.715277777781</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="32">
         <f t="shared" si="1"/>
         <v>4.1666666671517305E-2</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="36">
         <f>SUM(E14:E18)</f>
         <v>0.25694444444525288</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+      <c r="A19" s="19">
         <v>5</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="28">
         <v>45471.375</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="28">
         <v>45471.402777777781</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="22">
         <f t="shared" si="1"/>
         <v>2.7777777781011537E-2</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
+      <c r="A20" s="6">
         <v>5</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="12">
         <v>45471.402777777781</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="12">
         <v>45471.430555555555</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="8">
         <f t="shared" si="1"/>
         <v>2.7777777773735579E-2</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
         <v>5</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="12">
         <v>45471.430555555555</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="12">
         <v>45471.479166666664</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="8">
         <f t="shared" si="1"/>
         <v>4.8611111109494232E-2</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
         <v>5</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="12">
         <v>45471.479166666664</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="12">
         <v>45471.5625</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="8">
         <f>D22-C22</f>
         <v>8.3333333335758653E-2</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
         <v>5</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="12">
         <v>45471.645833333336</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="12">
         <v>45471.694444444445</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="8">
         <f>D23-C23</f>
         <v>4.8611111109494232E-2</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
         <v>5</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="31">
         <v>45471.694444444445</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="31">
         <v>45471.743055555555</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="32">
         <f>D24-C24</f>
         <v>4.8611111109494232E-2</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="36">
         <f>SUM(E19:E24)</f>
         <v>0.28472222221898846</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
+    <row r="25" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="19">
         <v>6</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="28">
         <v>45472.375</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="28">
         <v>45472.416666666664</v>
       </c>
-      <c r="E25" s="11">
-        <f t="shared" ref="E25:E34" si="2">D25-C25</f>
+      <c r="E25" s="22">
+        <f t="shared" ref="E25:E39" si="2">D25-C25</f>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
         <v>6</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="12">
         <v>45472.416666666664</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="12">
         <v>45472.465277777781</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="8">
         <f t="shared" si="2"/>
         <v>4.8611111116770189E-2</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>6</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="12">
         <v>45472.465277777781</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="12">
         <v>45472.527777777781</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="8">
         <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9">
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>6</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="12">
         <v>45472.527777777781</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="12">
         <v>45472.590277777781</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="8">
         <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:7" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
         <v>6</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="12">
         <v>45472.590277777781</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="12">
         <v>45472.631944444445</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="8">
         <f t="shared" si="2"/>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29">
         <v>6</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="31">
         <v>45472.666666666664</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="31">
         <v>45472.777777777781</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="32">
         <f t="shared" si="2"/>
         <v>0.11111111111677019</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="21">
+      <c r="G30" s="36">
         <f>SUM(E25:E30)</f>
         <v>0.36805555556202307</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9">
+    <row r="31" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="19">
         <v>7</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="28">
         <v>45474.375</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="28">
         <v>45474.444444444445</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="22">
         <f t="shared" si="2"/>
         <v>6.9444444445252884E-2</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
+      <c r="G31" s="23"/>
+    </row>
+    <row r="32" spans="1:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
         <v>7</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="12">
         <v>45474.444444444445</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="12">
         <v>45474.520833333336</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="8">
         <f t="shared" si="2"/>
         <v>7.6388888890505768E-2</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="10"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9">
+      <c r="A33" s="6">
         <v>7</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="12">
         <v>45474.520833333336</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="12">
         <v>45474.548611111109</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="8">
         <f t="shared" si="2"/>
         <v>2.7777777773735579E-2</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9">
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="29">
         <v>7</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="31">
         <v>45474.625</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="31">
         <v>45474.722222222219</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="32">
         <f t="shared" si="2"/>
         <v>9.7222222218988463E-2</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="36">
         <f>SUM(E31:E34)</f>
         <v>0.27083333332848269</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="13"/>
-      <c r="F35" s="13"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="13"/>
-      <c r="F36" s="13"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="13"/>
-      <c r="F37" s="13"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="13"/>
-      <c r="F38" s="13"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="13"/>
-      <c r="F39" s="13"/>
+    <row r="35" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="19">
+        <v>8</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="28">
+        <v>45475.375</v>
+      </c>
+      <c r="D35" s="28">
+        <v>45475.423611111109</v>
+      </c>
+      <c r="E35" s="22">
+        <f t="shared" si="2"/>
+        <v>4.8611111109494232E-2</v>
+      </c>
+      <c r="F35" s="42"/>
+      <c r="G35" s="23"/>
+    </row>
+    <row r="36" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>8</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="12">
+        <v>45475.423611111109</v>
+      </c>
+      <c r="D36" s="12">
+        <v>45475.493055555555</v>
+      </c>
+      <c r="E36" s="8">
+        <f t="shared" si="2"/>
+        <v>6.9444444445252884E-2</v>
+      </c>
+      <c r="F36" s="40"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>8</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="12">
+        <v>45475.493055555555</v>
+      </c>
+      <c r="D37" s="12">
+        <v>45475.534722222219</v>
+      </c>
+      <c r="E37" s="8">
+        <f t="shared" si="2"/>
+        <v>4.1666666664241347E-2</v>
+      </c>
+      <c r="F37" s="40"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>8</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="12">
+        <v>45475.618055555555</v>
+      </c>
+      <c r="D38" s="12">
+        <v>45475.680555555555</v>
+      </c>
+      <c r="E38" s="8">
+        <f t="shared" si="2"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F38" s="40"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="41">
+        <v>8</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="31">
+        <v>45475.722222222219</v>
+      </c>
+      <c r="D39" s="31">
+        <v>45475.8125</v>
+      </c>
+      <c r="E39" s="32">
+        <f t="shared" si="2"/>
+        <v>9.0277777781011537E-2</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="G39" s="36">
+        <f>SUM(E35:E39)</f>
+        <v>0.3125</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="B40" s="10"/>
+      <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="B41" s="10"/>
+      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="B42" s="10"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="24"/>
-      <c r="F43" s="13"/>
+      <c r="B43" s="18"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="24"/>
-      <c r="F44" s="13"/>
+      <c r="B44" s="18"/>
+      <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F45" s="13"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F46" s="13"/>
+      <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F47" s="13"/>
+      <c r="F47" s="10"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F48" s="13"/>
+      <c r="F48" s="10"/>
     </row>
     <row r="49" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F49" s="13"/>
+      <c r="F49" s="10"/>
     </row>
     <row r="50" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F50" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F2CB36-37D6-4F5C-A5E8-8F0B95A87B2D}">
-  <dimension ref="A6:A78"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="25" t="s">
-        <v>83</v>
-      </c>
+      <c r="F50" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final word and excel repots & final commit
</commit_message>
<xml_diff>
--- a/2024-УП-task_time_manager_2гр_Большаков.xlsx
+++ b/2024-УП-task_time_manager_2гр_Большаков.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\UP\AB_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C12E46-8E17-47A0-8C96-3F5B379E4CB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3905C8-AE09-4C86-8595-14D06C521BF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="28770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManager" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>№ за день</t>
   </si>
@@ -1528,8 +1528,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="102" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="102" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>3</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19">
         <v>4</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>45472.416666666664</v>
       </c>
       <c r="E25" s="22">
-        <f t="shared" ref="E25:E41" si="2">D25-C25</f>
+        <f t="shared" ref="E25:E40" si="2">D25-C25</f>
         <v>4.1666666664241347E-2</v>
       </c>
       <c r="F25" s="39" t="s">
@@ -2440,13 +2440,51 @@
         <v>0.35416666666424135</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="10"/>
-      <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="10"/>
-      <c r="F42" s="10"/>
+    <row r="41" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="43">
+        <v>10</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="45">
+        <v>45478.375</v>
+      </c>
+      <c r="D41" s="45">
+        <v>45478.708333333336</v>
+      </c>
+      <c r="E41" s="46">
+        <f t="shared" ref="E41:E42" si="3">D41-C41</f>
+        <v>0.33333333333575865</v>
+      </c>
+      <c r="F41" s="47"/>
+      <c r="G41" s="48">
+        <f>SUM(E41)</f>
+        <v>0.33333333333575865</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="43">
+        <v>11</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="45">
+        <v>45478.375</v>
+      </c>
+      <c r="D42" s="45">
+        <v>45478.625</v>
+      </c>
+      <c r="E42" s="46">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="F42" s="47"/>
+      <c r="G42" s="48">
+        <f>SUM(E42)</f>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="18"/>

</xml_diff>